<commit_message>
Eliminar porcentaje de crecimiento en inventarios, eliminar botón 'Nueva con Año' en bitácoras, y cambiar servicio Excel a producción
- Eliminado porcentaje de crecimiento de inventarios en dashboard (admin y login)
- Eliminado botón 'Nueva con Año' en pantalla de bitácoras (móvil y desktop)
- Cambiado servicio de exportación Excel a URL de producción (Render)
- Eliminada función _showAddBitacoraWithYearDialog no utilizada
</commit_message>
<xml_diff>
--- a/assets/plantilla_inventario_computo.xlsx
+++ b/assets/plantilla_inventario_computo.xlsx
@@ -158,6 +158,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -230,13 +231,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.25"/>
-        <bgColor rgb="FF1F497D"/>
+        <bgColor rgb="FF18A303"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF666699"/>
-        <bgColor rgb="FF376092"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
     <fill>
@@ -248,13 +249,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.25"/>
-        <bgColor rgb="FF1F497D"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.25"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
     <fill>
@@ -270,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -340,6 +341,41 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -348,10 +384,8 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right/>
-      <top style="thick">
-        <color theme="0"/>
-      </top>
+      <right style="thin"/>
+      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -384,7 +418,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -513,14 +547,38 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -529,10 +587,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -541,20 +595,32 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
@@ -567,11 +633,11 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Excel Built-in Heading 1" xfId="20"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF376092"/>
+          <fgColor rgb="FF127A02"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -642,15 +708,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF17375E"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF77933C"/>
+          <fgColor rgb="FF7A2E02"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -667,20 +725,20 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF127A02"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF77933C"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF4F81BD"/>
+      <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF376092"/>
+      <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFFFCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -706,13 +764,13 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF17375E"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF18A303"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF7A2E02"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF1F497D"/>
+      <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -730,9 +788,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>808560</xdr:colOff>
+      <xdr:colOff>808200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -746,7 +804,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="123840"/>
-          <a:ext cx="1656360" cy="442080"/>
+          <a:ext cx="1656000" cy="441720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -874,7 +932,7 @@
   </sheetPr>
   <dimension ref="A1:AN1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -893,20 +951,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="28.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="25.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="61.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="61.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="21.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="16.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="28.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="18.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="17.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="19.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="30.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="148.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="148.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1047,7 +1105,7 @@
       <c r="AM3" s="20"/>
       <c r="AN3" s="11"/>
     </row>
-    <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
@@ -1176,11 +1234,11 @@
       <c r="D5" s="34"/>
       <c r="E5" s="32"/>
       <c r="F5" s="32"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
       <c r="L5" s="32"/>
       <c r="M5" s="32"/>
       <c r="N5" s="32"/>
@@ -1195,147 +1253,147 @@
       <c r="W5" s="32"/>
       <c r="X5" s="32"/>
       <c r="Y5" s="32"/>
-      <c r="Z5" s="37"/>
+      <c r="Z5" s="36"/>
       <c r="AA5" s="32"/>
       <c r="AB5" s="32"/>
       <c r="AC5" s="32"/>
       <c r="AD5" s="32"/>
       <c r="AE5" s="32"/>
       <c r="AF5" s="32"/>
-      <c r="AG5" s="38"/>
+      <c r="AG5" s="37"/>
       <c r="AH5" s="32"/>
       <c r="AI5" s="32"/>
       <c r="AJ5" s="32"/>
       <c r="AK5" s="32"/>
       <c r="AL5" s="32"/>
       <c r="AM5" s="32"/>
-      <c r="AN5" s="35"/>
+      <c r="AN5" s="38"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="33"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="37"/>
-      <c r="AA6" s="32"/>
-      <c r="AB6" s="32"/>
-      <c r="AC6" s="32"/>
-      <c r="AD6" s="32"/>
-      <c r="AE6" s="32"/>
-      <c r="AF6" s="32"/>
-      <c r="AG6" s="38"/>
-      <c r="AH6" s="32"/>
-      <c r="AI6" s="32"/>
-      <c r="AJ6" s="32"/>
-      <c r="AK6" s="32"/>
-      <c r="AL6" s="32"/>
-      <c r="AM6" s="32"/>
-      <c r="AN6" s="32"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="42"/>
+      <c r="AA6" s="39"/>
+      <c r="AB6" s="39"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="39"/>
+      <c r="AE6" s="39"/>
+      <c r="AF6" s="39"/>
+      <c r="AG6" s="43"/>
+      <c r="AH6" s="39"/>
+      <c r="AI6" s="39"/>
+      <c r="AJ6" s="39"/>
+      <c r="AK6" s="39"/>
+      <c r="AL6" s="39"/>
+      <c r="AM6" s="39"/>
+      <c r="AN6" s="44"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="31"/>
-      <c r="B7" s="32"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="37"/>
-      <c r="AA7" s="32"/>
-      <c r="AB7" s="32"/>
-      <c r="AC7" s="32"/>
-      <c r="AD7" s="32"/>
-      <c r="AE7" s="32"/>
-      <c r="AF7" s="32"/>
-      <c r="AG7" s="38"/>
-      <c r="AH7" s="32"/>
-      <c r="AI7" s="32"/>
-      <c r="AJ7" s="32"/>
-      <c r="AK7" s="32"/>
-      <c r="AL7" s="32"/>
-      <c r="AM7" s="32"/>
-      <c r="AN7" s="32"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="39"/>
+      <c r="X7" s="39"/>
+      <c r="Y7" s="39"/>
+      <c r="Z7" s="42"/>
+      <c r="AA7" s="39"/>
+      <c r="AB7" s="39"/>
+      <c r="AC7" s="39"/>
+      <c r="AD7" s="39"/>
+      <c r="AE7" s="39"/>
+      <c r="AF7" s="39"/>
+      <c r="AG7" s="43"/>
+      <c r="AH7" s="39"/>
+      <c r="AI7" s="39"/>
+      <c r="AJ7" s="39"/>
+      <c r="AK7" s="39"/>
+      <c r="AL7" s="39"/>
+      <c r="AM7" s="39"/>
+      <c r="AN7" s="44"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31"/>
-      <c r="B8" s="39"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="39"/>
-      <c r="X8" s="39"/>
-      <c r="Y8" s="39"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="39"/>
-      <c r="AB8" s="39"/>
-      <c r="AC8" s="39"/>
-      <c r="AD8" s="39"/>
-      <c r="AE8" s="39"/>
-      <c r="AF8" s="39"/>
-      <c r="AG8" s="42"/>
-      <c r="AH8" s="39"/>
-      <c r="AI8" s="39"/>
-      <c r="AJ8" s="39"/>
-      <c r="AK8" s="39"/>
-      <c r="AL8" s="39"/>
-      <c r="AM8" s="39"/>
-      <c r="AN8" s="39"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="45"/>
+      <c r="X8" s="45"/>
+      <c r="Y8" s="45"/>
+      <c r="Z8" s="48"/>
+      <c r="AA8" s="45"/>
+      <c r="AB8" s="45"/>
+      <c r="AC8" s="45"/>
+      <c r="AD8" s="45"/>
+      <c r="AE8" s="45"/>
+      <c r="AF8" s="45"/>
+      <c r="AG8" s="49"/>
+      <c r="AH8" s="45"/>
+      <c r="AI8" s="45"/>
+      <c r="AJ8" s="45"/>
+      <c r="AK8" s="45"/>
+      <c r="AL8" s="45"/>
+      <c r="AM8" s="45"/>
+      <c r="AN8" s="50"/>
     </row>
     <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1421,47 +1479,47 @@
   </mergeCells>
   <dataValidations count="11">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="E5:E8" type="list">
-      <formula1>#¿NOMBRE?</formula1>
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H6:H8" type="list">
-      <formula1>#¿NOMBRE?</formula1>
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="Indicar valor de lista desplegable" errorStyle="stop" errorTitle="Validar información" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L5:M8" type="list">
-      <formula1>#¿NOMBRE?</formula1>
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="Indicar valor de lista desplegable" errorStyle="stop" errorTitle="Validar información" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N5:N8" type="list">
-      <formula1>#¿NOMBRE?</formula1>
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="Ingresar registro de lista desplegable" errorStyle="stop" errorTitle="Validar información" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R5:R8" type="list">
-      <formula1>#¿NOMBRE?</formula1>
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="Indicar dato de lista desplegable" errorStyle="stop" errorTitle="Validar información" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T5:T8" type="list">
-      <formula1>#¿NOMBRE?</formula1>
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="Indicar un valor de lista desplegable" errorStyle="stop" errorTitle="Verificar Estatus" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V5:V8" type="list">
-      <formula1>#¿NOMBRE?</formula1>
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="W5:W8" type="list">
-      <formula1>#¿NOMBRE?</formula1>
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="X5:X8" type="list">
-      <formula1>INDIRECT(#REF!)</formula1>
+      <formula1>INDIRECT(#ref!)</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="Indicar valor de lista desplegable" errorStyle="stop" errorTitle="Validad información" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AE5:AE8 AL5:AL8" type="list">
-      <formula1>#¿NOMBRE?</formula1>
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="Indicar valor de lista desplegable" errorStyle="stop" errorTitle="Validar dato" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AF5:AF8 AM5:AM8" type="list">
-      <formula1>#¿NOMBRE?</formula1>
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>